<commit_message>
Added Barchart to spreadsheet
</commit_message>
<xml_diff>
--- a/transaction2.xlsx
+++ b/transaction2.xlsx
@@ -1,131 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
-</workbook>
-</file>
-
-<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
-  <fonts count="1">
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
-</styleSheet>
-</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -423,7 +295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -431,7 +303,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -456,6 +328,11 @@
           <t>price</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -501,5 +378,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>